<commit_message>
Entrega Final Reto 1
</commit_message>
<xml_diff>
--- a/Docs/EntregaFinal_GráficasReto1.xlsx
+++ b/Docs/EntregaFinal_GráficasReto1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Desktop/ESTRUCTURA DE DATOS/LABORATORIOS/Reto1-G07/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8207E7-EB0D-CB49-BC07-8D8B38687EEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672C24BA-63AB-7742-A4A7-C59B94861980}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C3A23091-F56B-764B-B2A9-16EB20C813B3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabla datos" sheetId="1" r:id="rId1"/>
+    <sheet name="Tablas datos" sheetId="1" r:id="rId1"/>
     <sheet name="Requerimiento 0" sheetId="6" r:id="rId2"/>
     <sheet name="Requerimiento 1" sheetId="5" r:id="rId3"/>
     <sheet name="Requerimiento 2" sheetId="4" r:id="rId4"/>
@@ -30,12 +30,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
-    <t>Tamaño archivo CSV</t>
+    <t>Reuerimiento 0</t>
   </si>
   <si>
-    <t>Tiempo</t>
+    <t>Tamaño CSV [%]</t>
+  </si>
+  <si>
+    <t>Tiempo [s]</t>
+  </si>
+  <si>
+    <t>Reuerimiento 1</t>
+  </si>
+  <si>
+    <t>Reuerimiento 2</t>
+  </si>
+  <si>
+    <t>Reuerimiento 3</t>
+  </si>
+  <si>
+    <t>Reuerimiento 4</t>
   </si>
 </sst>
 </file>
@@ -71,32 +86,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -107,17 +106,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6096BAC3-887A-844F-90CB-810F657B76DF}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B5" xr:uid="{168CA342-B63F-1544-AD51-FCB65F1BC3D4}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DC1D5AA1-1D3C-384E-B7B4-E400FE60972E}" name="Tamaño archivo CSV" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{4499EA9F-5839-CC43-8846-DB627F919AC5}" name="Tiempo" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,56 +405,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D95D59-74F9-7A44-AA66-EE231A1E46A5}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>0.8</v>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>10</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="1">
+        <v>80</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>80</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="1">
+        <v>80</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>100</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="1">
+        <v>100</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>80</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>100</v>
+      </c>
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>